<commit_message>
working on filters for sfb
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -852,31 +852,31 @@
         <v>3607892</v>
       </c>
       <c r="H8" t="n">
-        <v>179267</v>
+        <v>179317</v>
       </c>
       <c r="I8" t="n">
         <v>25.97</v>
       </c>
       <c r="J8" t="n">
-        <v>4656339</v>
+        <v>4657659</v>
       </c>
       <c r="K8" t="n">
-        <v>320923</v>
+        <v>320973</v>
       </c>
       <c r="L8" t="n">
         <v>25.75</v>
       </c>
       <c r="M8" t="n">
-        <v>8264231</v>
+        <v>8265551</v>
       </c>
       <c r="N8" t="n">
-        <v>314496</v>
+        <v>234395</v>
       </c>
       <c r="O8" t="n">
-        <v>23.97</v>
+        <v>29.73</v>
       </c>
       <c r="P8" t="n">
-        <v>7538984</v>
+        <v>6967932</v>
       </c>
     </row>
     <row r="9">
@@ -1008,31 +1008,31 @@
         <v>5766237</v>
       </c>
       <c r="H11" t="n">
-        <v>312777</v>
+        <v>312827</v>
       </c>
       <c r="I11" t="n">
         <v>21.59</v>
       </c>
       <c r="J11" t="n">
-        <v>6753285</v>
+        <v>6754605</v>
       </c>
       <c r="K11" t="n">
-        <v>600396</v>
+        <v>600446</v>
       </c>
       <c r="L11" t="n">
         <v>20.85</v>
       </c>
       <c r="M11" t="n">
-        <v>12519522</v>
+        <v>12520842</v>
       </c>
       <c r="N11" t="n">
-        <v>314496</v>
+        <v>234395</v>
       </c>
       <c r="O11" t="n">
-        <v>23.97</v>
+        <v>29.73</v>
       </c>
       <c r="P11" t="n">
-        <v>7538984</v>
+        <v>6967932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>